<commit_message>
Added blue cell H4
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -34,7 +34,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,6 +44,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -60,9 +66,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H2"/>
+  <dimension ref="H2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -354,6 +361,9 @@
     <row r="2" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H2" s="1"/>
     </row>
+    <row r="4" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added purple cell H4
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -34,7 +34,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,6 +44,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -60,9 +66,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H2"/>
+  <dimension ref="H2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -354,6 +361,9 @@
     <row r="2" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H2" s="1"/>
     </row>
+    <row r="4" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added black cell H4
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -34,7 +34,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -44,6 +44,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -60,9 +66,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -343,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H2"/>
+  <dimension ref="H2:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -354,6 +361,9 @@
     <row r="2" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H2" s="1"/>
     </row>
+    <row r="4" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>